<commit_message>
- Fixed bugs in Practice registry - Fixed bugs in Provider registry - Some GUI bugs fix - Some Analytics bug fix
</commit_message>
<xml_diff>
--- a/assets/SchemaForAllWorksheets.xlsx
+++ b/assets/SchemaForAllWorksheets.xlsx
@@ -456,17 +456,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Optum Care Arizona</t>
+          <t>Echelon Care Organisation</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -493,17 +493,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4900</t>
+          <t>200</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Optum Care Network Washington</t>
+          <t>Enlighten Care Organisation</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -530,17 +530,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SCPMCS</t>
+          <t>Excalibur Physicians Association</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -567,17 +567,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4600</t>
+          <t>6500</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MedPOINT Management</t>
+          <t>Guardian Care Delivery Organisation</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -604,17 +604,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5800</t>
+          <t>1100</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Stanford Health Care</t>
+          <t>Saint Care Delivery Organisation</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">

</xml_diff>